<commit_message>
mise a jour du rapport avec les test de perfs
Signed-off-by: Nicolas <nicolas.droesch@gmail.com>
</commit_message>
<xml_diff>
--- a/Resultat_tests.xlsx
+++ b/Resultat_tests.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atlas\PycharmProjects\BC_CO2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E661D87-5FA4-40DF-801E-D534367AAC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F876914-76B4-4F6A-90FD-1C2483F97ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{F3F7CF39-7817-4C81-A1C9-8C7B4E910B7C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F3F7CF39-7817-4C81-A1C9-8C7B4E910B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>énergie</t>
   </si>
@@ -85,6 +84,24 @@
   </si>
   <si>
     <t>TestCases</t>
+  </si>
+  <si>
+    <t>Testcase</t>
+  </si>
+  <si>
+    <t>Energie</t>
+  </si>
+  <si>
+    <t>10 utilisateurs/minute, vent, intensité change toutes les minutes</t>
+  </si>
+  <si>
+    <t>100 utilisateurs/minute, vent, intensité change toutes les minutes</t>
+  </si>
+  <si>
+    <t>1000 utilisateurs/minute, vent, intensité change toutes les minutes</t>
+  </si>
+  <si>
+    <t>1000 utilisateurs/minute en rajoutant un cache (lrucache ? via le navigateur ?)</t>
   </si>
 </sst>
 </file>
@@ -106,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +139,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -153,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -167,13 +196,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -510,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C1AB97-FE0A-44BF-8A9B-F6BB901464E8}">
-  <dimension ref="D7:I15"/>
+  <dimension ref="D7:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:I15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,54 +561,73 @@
     <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="62.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D7" s="5" t="s">
+    <row r="7" spans="4:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="9" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="K7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
       <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="K8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="6">
+        <v>4.8148827837807602E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
       <c r="I9" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="K9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="1">
+        <v>6.9419456519546098E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" ht="30" x14ac:dyDescent="0.25">
       <c r="D10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>4.7824000000105104E-7</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>4.9297222222182599E-9</v>
       </c>
       <c r="G10" s="2">
@@ -586,15 +640,21 @@
       <c r="I10" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="K10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="1">
+        <v>8.0519174630830206E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12" ht="30" x14ac:dyDescent="0.25">
       <c r="D11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>5.4910999999719899E-7</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>6.2827777777367004E-9</v>
       </c>
       <c r="G11" s="2">
@@ -607,15 +667,21 @@
       <c r="I11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="K11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.236150452437773</v>
+      </c>
+    </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="2">
         <v>1.24752899999998E-4</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>3.45495944444438E-6</v>
       </c>
       <c r="G12" s="2">
@@ -629,35 +695,35 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>4.55269999997653E-7</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>3.3669444443754999E-9</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
         <v>4.586369444420285E-7</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>2.4080276489257799E-5</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:12" ht="45" x14ac:dyDescent="0.25">
       <c r="D14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>5.8388999996168401E-7</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>5.0919444434940498E-9</v>
       </c>
       <c r="G14" s="2">
@@ -671,14 +737,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:12" ht="45" x14ac:dyDescent="0.25">
       <c r="D15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>8.3614000000124998E-7</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>1.2773333332916E-8</v>
       </c>
       <c r="G15" s="2">

</xml_diff>